<commit_message>
final statement, started submitting
</commit_message>
<xml_diff>
--- a/Grad Schools.xlsx
+++ b/Grad Schools.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="60">
   <si>
     <t>School</t>
   </si>
@@ -147,10 +147,58 @@
     <t>UCSB</t>
   </si>
   <si>
-    <t>Just need statement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Correct dept GPA, JP description in Additional Academic Background, Applicants to the Departments of Astronomy and of Physics must submit in addition to this abstract, a list of their four most advanced courses in astronomy and physics and their two most advanced courses in mathematics, indicating textbooks (and authors) used in each course. </t>
+    <t xml:space="preserve">Applicants to the Departments of Astronomy and of Physics must submit in addition to this abstract, a list of their four most advanced courses in astronomy and physics and their two most advanced courses in mathematics, indicating textbooks (and authors) used in each course. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Just need </t>
+  </si>
+  <si>
+    <t>Test Scores</t>
+  </si>
+  <si>
+    <t>Economic, Statement, Personal history</t>
+  </si>
+  <si>
+    <t>Statement</t>
+  </si>
+  <si>
+    <t>Fischer, Langer, Ludwig</t>
+  </si>
+  <si>
+    <t>Financial, SOP, PS</t>
+  </si>
+  <si>
+    <t>SOP</t>
+  </si>
+  <si>
+    <t>Ehud Altman: Strongly Corr and Q infor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dung-Hai Lee: Novel phases </t>
+  </si>
+  <si>
+    <t>Yao: Topological phases</t>
+  </si>
+  <si>
+    <t>Alexei Kitaev: Topological quantum phases and computation</t>
+  </si>
+  <si>
+    <t>Leon Balents: Strongly correlated systems</t>
+  </si>
+  <si>
+    <t>Wim van Dam: Quantum information and computing</t>
+  </si>
+  <si>
+    <t>Mark Srednicki: Quantum chaos</t>
+  </si>
+  <si>
+    <t>Rahul Nandkishore: Emergent phenomena</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Victor Gurarie: Applications of quantum field theory to </t>
+  </si>
+  <si>
+    <t>Paul Beale: statistical mechanics of condensed matter systems</t>
   </si>
 </sst>
 </file>
@@ -208,8 +256,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="25">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -250,7 +300,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="25">
+  <cellStyles count="27">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -263,6 +313,7 @@
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -275,6 +326,7 @@
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -606,8 +658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="S9" sqref="S9"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0"/>
@@ -736,16 +788,19 @@
       <c r="R3" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="S3" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="T3" s="1" t="s">
         <v>33</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="30" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B4" s="4">
         <v>43084</v>
@@ -754,38 +809,32 @@
         <v>1</v>
       </c>
       <c r="D4" s="2">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2">
         <v>1</v>
       </c>
-      <c r="E4" s="2">
-        <v>4</v>
-      </c>
       <c r="F4" s="1">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G4" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="O4" s="1">
-        <v>3514</v>
-      </c>
       <c r="P4" s="1">
-        <v>75</v>
+        <v>105</v>
       </c>
       <c r="Q4" s="1" t="s">
         <v>17</v>
@@ -796,10 +845,13 @@
       <c r="T4" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="U4" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="5" spans="1:21" ht="30" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="4">
         <v>43084</v>
@@ -808,18 +860,39 @@
         <v>1</v>
       </c>
       <c r="D5" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E5" s="2">
+        <v>4</v>
+      </c>
+      <c r="F5" s="1">
         <v>3</v>
       </c>
-      <c r="F5" s="1">
-        <v>4</v>
-      </c>
       <c r="G5" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H5" s="3"/>
+      <c r="I5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O5" s="1">
+        <v>3514</v>
+      </c>
+      <c r="P5" s="1">
+        <v>75</v>
+      </c>
       <c r="Q5" s="1" t="s">
         <v>17</v>
       </c>
@@ -827,32 +900,44 @@
         <v>17</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="30" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>41</v>
+        <v>5</v>
       </c>
       <c r="B6" s="4">
         <v>43084</v>
       </c>
       <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2">
+        <v>2</v>
+      </c>
+      <c r="E6" s="2">
+        <v>3</v>
+      </c>
+      <c r="F6" s="1">
         <v>4</v>
       </c>
-      <c r="D6" s="2">
-        <v>10</v>
-      </c>
-      <c r="E6" s="2">
-        <v>5</v>
-      </c>
-      <c r="F6" s="1">
-        <v>5</v>
-      </c>
       <c r="G6" s="3">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H6" s="3"/>
+      <c r="I6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="Q6" s="1" t="s">
         <v>17</v>
       </c>
@@ -860,46 +945,34 @@
         <v>17</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="30" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="4">
-        <v>43084</v>
+        <v>25</v>
       </c>
       <c r="C7" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D7" s="2">
         <v>2</v>
       </c>
       <c r="E7" s="2">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F7" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G7" s="3">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H7" s="3"/>
       <c r="I7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="P7" s="1">
-        <v>105</v>
+        <v>53</v>
       </c>
       <c r="Q7" s="1" t="s">
         <v>17</v>
@@ -908,32 +981,47 @@
         <v>17</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="U7" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="30" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>25</v>
+        <v>41</v>
+      </c>
+      <c r="B8" s="4">
+        <v>43084</v>
       </c>
       <c r="C8" s="2">
         <v>4</v>
       </c>
       <c r="D8" s="2">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E8" s="2">
+        <v>5</v>
+      </c>
+      <c r="F8" s="1">
+        <v>5</v>
+      </c>
+      <c r="G8" s="3">
         <v>7</v>
       </c>
-      <c r="F8" s="1">
-        <v>9</v>
-      </c>
-      <c r="G8" s="3">
-        <v>6</v>
-      </c>
       <c r="H8" s="3"/>
+      <c r="I8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="Q8" s="1" t="s">
         <v>17</v>
       </c>
@@ -941,7 +1029,10 @@
         <v>17</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="30" customHeight="1">
@@ -952,6 +1043,15 @@
         <v>43084</v>
       </c>
       <c r="D9" s="2"/>
+      <c r="I9" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="N9" s="1" t="s">
         <v>18</v>
       </c>
@@ -967,9 +1067,9 @@
       <c r="R9" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:21" ht="30" customHeight="1">
-      <c r="D10" s="2"/>
+      <c r="U9" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="11" spans="1:21" ht="30" customHeight="1">
       <c r="D11" s="2"/>

</xml_diff>

<commit_message>
Starting again in 2018
</commit_message>
<xml_diff>
--- a/Grad Schools.xlsx
+++ b/Grad Schools.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="55">
   <si>
     <t>School</t>
   </si>
@@ -69,9 +69,6 @@
     <t>Started?</t>
   </si>
   <si>
-    <t>Finished?</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -147,30 +144,9 @@
     <t>UCSB</t>
   </si>
   <si>
-    <t xml:space="preserve">Applicants to the Departments of Astronomy and of Physics must submit in addition to this abstract, a list of their four most advanced courses in astronomy and physics and their two most advanced courses in mathematics, indicating textbooks (and authors) used in each course. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Just need </t>
-  </si>
-  <si>
-    <t>Test Scores</t>
-  </si>
-  <si>
-    <t>Economic, Statement, Personal history</t>
-  </si>
-  <si>
-    <t>Statement</t>
-  </si>
-  <si>
     <t>Fischer, Langer, Ludwig</t>
   </si>
   <si>
-    <t>Financial, SOP, PS</t>
-  </si>
-  <si>
-    <t>SOP</t>
-  </si>
-  <si>
     <t>Ehud Altman: Strongly Corr and Q infor</t>
   </si>
   <si>
@@ -199,6 +175,15 @@
   </si>
   <si>
     <t>Paul Beale: statistical mechanics of condensed matter systems</t>
+  </si>
+  <si>
+    <t>Submitted?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Scores Received?</t>
   </si>
 </sst>
 </file>
@@ -256,8 +241,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="27">
+  <cellStyleXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -300,7 +289,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="27">
+  <cellStyles count="31">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -314,6 +303,8 @@
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -327,6 +318,8 @@
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -656,37 +649,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U13"/>
+  <dimension ref="A1:AB13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="9" style="1" customWidth="1"/>
     <col min="2" max="2" width="9.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5" style="2" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5" style="1" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5" style="2" hidden="1" customWidth="1"/>
-    <col min="6" max="7" width="18.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5" style="2" customWidth="1"/>
+    <col min="6" max="7" width="18.1640625" style="1" customWidth="1"/>
     <col min="8" max="8" width="1.83203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="28.33203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="23.6640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="25.83203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="25" style="1" customWidth="1"/>
+    <col min="10" max="10" width="20.1640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="24" style="1" customWidth="1"/>
     <col min="12" max="12" width="22.33203125" style="1" customWidth="1"/>
     <col min="13" max="13" width="10.83203125" style="1" customWidth="1"/>
     <col min="14" max="14" width="13.1640625" style="1" customWidth="1"/>
     <col min="15" max="15" width="9.33203125" style="1" customWidth="1"/>
     <col min="16" max="16" width="6" style="1" customWidth="1"/>
-    <col min="17" max="18" width="10.83203125" style="1" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="10.83203125" style="1" customWidth="1"/>
-    <col min="20" max="20" width="13.33203125" style="1" customWidth="1"/>
-    <col min="21" max="21" width="25.83203125" style="1" customWidth="1"/>
-    <col min="22" max="16384" width="10.83203125" style="1"/>
+    <col min="17" max="19" width="10.83203125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="13.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="14.83203125" style="1" customWidth="1"/>
+    <col min="22" max="22" width="25.83203125" style="1" customWidth="1"/>
+    <col min="23" max="27" width="10.83203125" style="1"/>
+    <col min="29" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="15" customHeight="1">
+    <row r="1" spans="1:22" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -694,10 +688,10 @@
         <v>7</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>8</v>
@@ -716,7 +710,7 @@
         <v>13</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>14</v>
@@ -725,28 +719,31 @@
         <v>15</v>
       </c>
       <c r="R1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="S1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" ht="15" customHeight="1">
+    </row>
+    <row r="2" spans="1:22" ht="15" customHeight="1">
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:21" ht="30" customHeight="1">
+    <row r="3" spans="1:22" ht="30" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="4">
-        <v>43081</v>
+        <v>43452</v>
       </c>
       <c r="C3" s="2">
         <v>4</v>
@@ -774,7 +771,7 @@
         <v>12</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O3" s="1">
         <v>4704</v>
@@ -783,27 +780,24 @@
         <v>125</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" ht="30" customHeight="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="30" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="4">
-        <v>43084</v>
+        <v>43449</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
@@ -822,39 +816,42 @@
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="K4" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="N4" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="P4" s="1">
         <v>105</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="U4" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" ht="30" customHeight="1">
+        <v>33</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" ht="30" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="4">
-        <v>43084</v>
+        <v>43449</v>
       </c>
       <c r="C5" s="2">
         <v>1</v>
@@ -873,19 +870,19 @@
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="L5" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="N5" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O5" s="1">
         <v>3514</v>
@@ -894,25 +891,23 @@
         <v>75</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="U5" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" ht="30" customHeight="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="30" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="4">
-        <v>43084</v>
-      </c>
+      <c r="B6" s="4"/>
       <c r="C6" s="2">
         <v>1</v>
       </c>
@@ -930,30 +925,33 @@
       </c>
       <c r="H6" s="3"/>
       <c r="I6" s="1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="U6" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" ht="30" customHeight="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" ht="30" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="B7" s="4">
+        <v>43449</v>
       </c>
       <c r="C7" s="2">
         <v>4</v>
@@ -972,27 +970,27 @@
       </c>
       <c r="H7" s="3"/>
       <c r="I7" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="U7" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" ht="30" customHeight="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" ht="30" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B8" s="4">
-        <v>43084</v>
+        <v>43449</v>
       </c>
       <c r="C8" s="2">
         <v>4</v>
@@ -1011,49 +1009,49 @@
       </c>
       <c r="H8" s="3"/>
       <c r="I8" s="1" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="U8" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" ht="30" customHeight="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" ht="30" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B9" s="4">
-        <v>43084</v>
+        <v>43449</v>
       </c>
       <c r="D9" s="2"/>
       <c r="I9" s="1" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="O9" s="1">
         <v>4841</v>
@@ -1062,22 +1060,22 @@
         <v>60</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="U9" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" ht="30" customHeight="1">
+        <v>16</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" ht="30" customHeight="1">
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:21" ht="30" customHeight="1">
+    <row r="12" spans="1:22" ht="30" customHeight="1">
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:21" ht="30" customHeight="1">
+    <row r="13" spans="1:22" ht="30" customHeight="1">
       <c r="D13" s="2"/>
     </row>
   </sheetData>

</xml_diff>